<commit_message>
Added a new version
</commit_message>
<xml_diff>
--- a/Assignment/MT103_analysis.xlsx
+++ b/Assignment/MT103_analysis.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\School\Master in Digital Driven Business - AUAS Amsterdam\Q3\1. Fintech Systems dev\Assignment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C23C84-329D-46B7-9974-05BC8E200CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
   <si>
     <t>transaction_date</t>
   </si>
@@ -118,7 +124,31 @@
     <t>highRisk</t>
   </si>
   <si>
-    <t>ComplFATF</t>
+    <t>within_date_thres</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>within_cd_thres</t>
+  </si>
+  <si>
+    <t>within_amount_thres</t>
+  </si>
+  <si>
+    <t>Smurfing</t>
+  </si>
+  <si>
+    <t>FATFCompl</t>
+  </si>
+  <si>
+    <t>ShellComp</t>
+  </si>
+  <si>
+    <t>susCountryRouting</t>
+  </si>
+  <si>
+    <t>vague_Paym_Msg</t>
   </si>
   <si>
     <t>example_1.txt</t>
@@ -229,7 +259,7 @@
     <t>METRO BANK PLC</t>
   </si>
   <si>
-    <t>HSBC HONG KONG</t>
+    <t>HSBCHKHHHKXXX</t>
   </si>
   <si>
     <t>LONDON, UNITED KINGDOM</t>
@@ -310,11 +340,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +408,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -424,7 +462,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -456,9 +494,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -490,6 +546,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -665,14 +739,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AR4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AI3" sqref="AI3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="50" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -778,91 +900,115 @@
       <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2">
         <v>44641</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="O2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="P2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="R2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="S2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="T2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="U2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="V2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="W2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="X2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="Z2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AA2" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="AB2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="AC2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="AD2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="AE2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="AF2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="AG2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="AH2" t="b">
         <v>1</v>
@@ -873,91 +1019,115 @@
       <c r="AJ2" t="b">
         <v>0</v>
       </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AL2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2">
         <v>44641</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="L3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="N3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="O3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="P3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R3" t="s">
+        <v>73</v>
+      </c>
+      <c r="S3" t="s">
+        <v>76</v>
+      </c>
+      <c r="T3" t="s">
+        <v>79</v>
+      </c>
+      <c r="U3" t="s">
+        <v>81</v>
+      </c>
+      <c r="V3" t="s">
+        <v>82</v>
+      </c>
+      <c r="W3" t="s">
+        <v>85</v>
+      </c>
+      <c r="X3" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z3" t="s">
         <v>60</v>
       </c>
-      <c r="Q3" t="s">
-        <v>63</v>
-      </c>
-      <c r="R3" t="s">
-        <v>65</v>
-      </c>
-      <c r="S3" t="s">
-        <v>68</v>
-      </c>
-      <c r="T3" t="s">
-        <v>71</v>
-      </c>
-      <c r="U3" t="s">
-        <v>73</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="AA3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD3" t="s">
         <v>74</v>
       </c>
-      <c r="W3" t="s">
-        <v>77</v>
-      </c>
-      <c r="X3" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>66</v>
-      </c>
       <c r="AE3" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="AF3" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="AG3" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="AH3" t="b">
         <v>1</v>
@@ -968,97 +1138,121 @@
       <c r="AJ3" t="b">
         <v>0</v>
       </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2">
         <v>44641</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L4" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="N4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="O4" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="P4" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="Q4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="R4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="S4" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="T4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="U4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="V4" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="W4" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="X4" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="Y4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="Z4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="AA4" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="AB4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="AC4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="AD4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="AE4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="AF4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="AG4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="AH4" t="b">
         <v>0</v>
@@ -1067,6 +1261,30 @@
         <v>0</v>
       </c>
       <c r="AJ4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>1</v>
+      </c>
+      <c r="AL4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR4" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>